<commit_message>
updated minor test run
testing db functionality on a small portion of the questions
</commit_message>
<xml_diff>
--- a/files/galen_allresults_grouped_by_model_db.xlsx
+++ b/files/galen_allresults_grouped_by_model_db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Model</t>
   </si>
@@ -46,47 +46,10 @@
     <t>Relationship between dependency scores of JAK1 in DepMapDB.</t>
   </si>
   <si>
-    <t>``` sql
- --  Ass uming  the  tables  are  named  as  ' gen es ',  ' samples ',  and  ' expression'
- --  With  the  following  schema:
- --  genes:  id  ( int ),  name  ( var char)
- --  samples:  id  ( int ),  sample_ type  ( var char)
- --  expression:  gene_ id  ( int ),  sample_ id  ( int ),  expression_ value  ( float)
- SELECT  g. name,  s. sample_ type,  AVG(e. expression_ value)  as  avg_ expression
- FROM  genes  g
- JO IN  expression  e  ON  g. id  =  e.g ene_ id
- JO IN  samples  s  ON  e. sample_ id  =  s. id
-W HERE  g. name  =  ' POLR3E'
- GROUP  BY  s. sample_ type
-H AV ING  s. sample_ type  IN  ('c ancer ',  ' normal ')
- ORDER  BY  s. sample_ type;
- --  Get  the  difference  in  expression  between  cancer  and  normal
- SELECT  'd iffer ential_ expression ',  name,  ( avg_ expression_c ancer  -  avg_ expression_ normal)  as  expression_d ifference
- FROM  (
-   SE LECT  g. name,  AVG(e. expression_ value)  as  avg_ expression_c ancer,  AVG( CASE  WH EN  s. sample_ type  =  'c ancer'  TH EN  e. expression_ value  EL SE  NULL  END)  as  avg_ expression_ normal
-   FROM  genes  g
-   JO IN  expression  e  ON  g. id  =  e.g ene_ id
-   JO IN  samples  s  ON  e. sample_ id  =  s. id
-   WHERE  g. name  =  ' POLR3E'
-   G RO UP  BY  s. sample_ type
-)  as  sub query
- ORDER  BY  expression_d ifference  DESC
- LIMIT 1;
- --  Det ermine  if  P OLR3E  is  over ex pressed  or  und erex pressed  in  cancer
- SELECT  CA SE
-   WH EN  expression_d ifference  &gt; 0  TH EN  ' over ex pressed'
-   EL SE  ' und erex pressed'
- END  as  expression_ status
- FROM  (
-   SE LECT  ( avg_ expression_c ancer  -  avg_ expression_ normal)  as  expression_d ifference
-   FROM  (
-      SE LECT  AVG(e. expression_ value)  as  avg_ expression_c ancer,  AVG( CASE  WH EN  s. sample</t>
-  </si>
-  <si>
-    <t>``` sql   -- Ass uming the tables are named" gen es "," prote ins ", and" mut ations"  -- and they have the following columns:  -- genes: id( int ), gene_ symbol( var char ), protein_ id( int)  -- prote ins: id( int ), protein_ id( int ), sequence( var char)  -- mut ations: id( int ), gene_ id( int ), position( int ), frequency( float)   -- This query calcul ates the mut ation frequency for each position in the protein sequence of geneP OLR3E  SELECTp. position AS position, AVG(m. frequency) AS avg_ frequency  FROM genesg  JO IN prote insp ONg. prote in_ id=p. id  JO IN mut ationsm ONg. id=m.g ene_ id W HEREg.g ene_ symbol=' POLR3E'  GROUP BYp. position   -- This query ident ifies positions witha mut ation frequency abovea certain threshold(e.g ., 0.05)  SET@ threshold= 0.05;   SELECTp. position AS position  FROM(   SE LECTp. position, AVG(m. frequency) AS avg_ frequency   FROM genesg   JO IN prote insp ONg. prote in_ id=p. id   JO IN mut ationsm ONg. id=m.g ene_ id   WHEREg.g ene_ symbol=' POLR3E'  G RO UP BYp. position )x W HERE avg_ frequency&gt;@ threshold;   '''   -- This query comb ines the previous two queries into one to find specific regions of the protein where mut ations occur ata higher frequency for geneP OLR3E.</t>
-  </si>
-  <si>
     <t>``` SQL   -- Ass uming the following table names and columns based on the given context  -- Table: prote ins( id, name, pas_ domain_ sequence)  -- Table: mut ations( id, protein_ id, position, type)  -- Table: cell_ lines( id, name, ic50)   -- First, join prote ins and mut ations tables using protein_ id  SELECTp. name AS protein_ name,m. position,m. type  FROM prote insp  JO IN mut ationsm ONp. id=m. prote in_ id W HEREp. name=' target_ prote in' -- replace with the actual protein name  ANDp. pas_ domain_ sequence IS NOT NULL -- assuming pas_ domain_ sequence is stored in prote ins table   -- Then, filter mut ations that are located inP AS domain  -- This assumes that the length ofP AS domain is known and stored ina variable or hardc oded value  -- Re place' start_ index' and' end_ index' with actual values  -- For example, if theP AS domain of the target protein is between positions 100 and 200:  ANDm. positionB ET WE EN start_ index AND end_ index   -- Join the result with cell_ lines table using ic50 values  -- Ass uming the select ivity is in vers ely proport ional to ic50, so lower ic50 values indicate higher select ivity for pro state cancer cell lines  -- Re place' pro state_ cell_ line_ id' with the actual id of the pro state cell line  SELECT protein_ name, position, type, ic50  FROM(   SE LECTp. name AS protein_ name,m. position,m. type   FROM prote insp   JO IN mut ationsm ONp. id=m. prote in_ id   WHEREp. name=' target_ prote in'   ANDp. pas_ domain_ sequence IS NOT NULL   ANDm. positionB ET WE EN start_ index AND end_ index ) mut ations  JO IN cell_ lines cl ON mut ations. id= cl. mut ation_ id -- assuming there isa mut ation_ id column in cell_ lines table W HERE cl. id= pro state_ cell_ line_ id  ORDER BY</t>
+  </si>
+  <si>
+    <t>```sql--JointheCCLE_GisticCNDBandCCLEMutDBtablesontheDepMap_IDcolumnforgenePOLR3ESELECTc.CCLE_Name,g.gistic_cnFROMccle_cn_gisticcJOINccle_mutationgONc.DepMap_ID=g.DepMap_IDWHEREHugo_Symbol='POLR3E';--Gettheabsolutevalueofgistic_cnandcheckifitissignificantlydifferentbetweencancerandnormaltissues--Thisqueryassumesthatthereisaseparatetableorcolumnthatindicatesthetissuetype(cancerornormal)foreachentryintheCCLE_GisticCNDBtable--Replace'tissue_type_table'and'tissue_type_column'withtheactualnamesofthetableandcolumnthatcontainthisinformation--Thisqueryalsoassumesthatthereisafunctionorwaytodetermineifthegeneisoverexpressedorunderexpressedbasedonthegistic_cnvalueDECLARE@POLR3E_gistic_cnVARCHAR(10);SET@POLR3E_gistic_cn=(SELECTABS(CAST(gistic_cnASINT))FROMccle_cn_gisticJOINccle_mutationmONccle_cn_gistic.DepMap_ID=ccle_mutation.DepMap_IDWHEREHugo_Symbol='POLR3E');SELECT'POLR3E'ASGene_Symbol,@POLR3E_gistic_cnASgistic_cn,(--ReplacethisquerywiththeactuallogictodetermineifthegeneisoverexpressedorunderexpressedCASEWHEN(SELECTCOUNT(*)FROMtissue_type_tableWHEREtissue_type='cancer'ANDDepMap_ID=c.DepMap_IDANDABS(CAST(gistic_cnASINT))&gt;(--ReplacethisquerywiththeactuallogictodeterminethethresholdforsignificantdifferentialexpressionSELECTAVG(ABS(CAST(gistic_cnASINT)))FROMtissue_type_tableWHEREtissue</t>
   </si>
 </sst>
 </file>
@@ -480,7 +443,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -513,7 +476,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -524,7 +487,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>